<commit_message>
Calibration FF and eta_is with scipy.optimize
</commit_message>
<xml_diff>
--- a/Python27/Calibration/Example_ExpData_R245FA.xlsx
+++ b/Python27/Calibration/Example_ExpData_R245FA.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="12">
   <si>
     <t>Refrigerant</t>
   </si>
@@ -41,6 +41,15 @@
   </si>
   <si>
     <t>'m_dot [Kg/s]'</t>
+  </si>
+  <si>
+    <t>T_su_exp [C]'</t>
+  </si>
+  <si>
+    <t>T_ex_exp [C]'</t>
+  </si>
+  <si>
+    <t>FillingFactor [-]'</t>
   </si>
 </sst>
 </file>
@@ -105,7 +114,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -152,6 +161,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H86"/>
+  <dimension ref="A1:K86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="J3" sqref="J3:J45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -471,9 +481,12 @@
     <col min="5" max="5" width="17.33203125" customWidth="1"/>
     <col min="6" max="6" width="17.21875" customWidth="1"/>
     <col min="8" max="8" width="16.5546875" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
+    <col min="10" max="10" width="14.77734375" customWidth="1"/>
+    <col min="11" max="11" width="16.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -498,8 +511,17 @@
       <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -531,8 +553,20 @@
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" s="1">
+        <f t="shared" ref="I2" si="3">H2+1</f>
+        <v>8</v>
+      </c>
+      <c r="J2" s="1">
+        <f t="shared" ref="J2" si="4">I2+1</f>
+        <v>9</v>
+      </c>
+      <c r="K2" s="1">
+        <f t="shared" ref="K2" si="5">J2+1</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -558,8 +592,17 @@
       <c r="H3" s="13">
         <v>0.16189999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3">
+        <v>123.8</v>
+      </c>
+      <c r="J3">
+        <v>96.09</v>
+      </c>
+      <c r="K3">
+        <v>1.3282595804632393</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -570,7 +613,7 @@
         <v>132215</v>
       </c>
       <c r="D4" s="5">
-        <f t="shared" ref="D4:D45" si="3">B4/C4</f>
+        <f t="shared" ref="D4:D45" si="6">B4/C4</f>
         <v>5.4650682600310105</v>
       </c>
       <c r="E4" s="5">
@@ -585,8 +628,17 @@
       <c r="H4" s="13">
         <v>0.1716</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4">
+        <v>123.9</v>
+      </c>
+      <c r="J4">
+        <v>95.88</v>
+      </c>
+      <c r="K4">
+        <v>1.3262314669790989</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -597,7 +649,7 @@
         <v>135481</v>
       </c>
       <c r="D5" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>5.6061366538481412</v>
       </c>
       <c r="E5" s="5">
@@ -612,8 +664,17 @@
       <c r="H5" s="13">
         <v>0.1812</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5">
+        <v>124</v>
+      </c>
+      <c r="J5">
+        <v>95.57</v>
+      </c>
+      <c r="K5">
+        <v>1.325009719740188</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
@@ -624,7 +685,7 @@
         <v>138519</v>
       </c>
       <c r="D6" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>5.7518896324691919</v>
       </c>
       <c r="E6" s="5">
@@ -639,8 +700,17 @@
       <c r="H6" s="13">
         <v>0.19089999999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6">
+        <v>124.1</v>
+      </c>
+      <c r="J6">
+        <v>95.23</v>
+      </c>
+      <c r="K6">
+        <v>1.3233005018304822</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
@@ -651,7 +721,7 @@
         <v>143420</v>
       </c>
       <c r="D7" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>5.8303026077255611</v>
       </c>
       <c r="E7" s="5">
@@ -666,8 +736,17 @@
       <c r="H7" s="13">
         <v>0.20119999999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7">
+        <v>124.2</v>
+      </c>
+      <c r="J7">
+        <v>95</v>
+      </c>
+      <c r="K7">
+        <v>1.3209070926354276</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
@@ -678,7 +757,7 @@
         <v>152276</v>
       </c>
       <c r="D8" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>6.2716186398381888</v>
       </c>
       <c r="E8" s="5">
@@ -693,8 +772,17 @@
       <c r="H8" s="13">
         <v>0.2334</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8">
+        <v>123.9</v>
+      </c>
+      <c r="J8">
+        <v>93.24</v>
+      </c>
+      <c r="K8">
+        <v>1.3132730458009894</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -705,7 +793,7 @@
         <v>155691</v>
       </c>
       <c r="D9" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>6.4486707645271721</v>
       </c>
       <c r="E9" s="5">
@@ -720,8 +808,17 @@
       <c r="H9" s="13">
         <v>0.24660000000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9">
+        <v>124</v>
+      </c>
+      <c r="J9">
+        <v>92.6</v>
+      </c>
+      <c r="K9">
+        <v>1.3089838283447142</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -732,7 +829,7 @@
         <v>162630</v>
       </c>
       <c r="D10" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>6.4440755088237101</v>
       </c>
       <c r="E10" s="5">
@@ -747,8 +844,17 @@
       <c r="H10" s="13">
         <v>0.25850000000000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10">
+        <v>124</v>
+      </c>
+      <c r="J10">
+        <v>92.28</v>
+      </c>
+      <c r="K10">
+        <v>1.3040754740747091</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -759,7 +865,7 @@
         <v>165685</v>
       </c>
       <c r="D11" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>6.5787488306123061</v>
       </c>
       <c r="E11" s="5">
@@ -774,8 +880,17 @@
       <c r="H11" s="13">
         <v>0.27039999999999997</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I11">
+        <v>124.2</v>
+      </c>
+      <c r="J11">
+        <v>91.83</v>
+      </c>
+      <c r="K11">
+        <v>1.3025191275066161</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -786,7 +901,7 @@
         <v>172083</v>
       </c>
       <c r="D12" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>6.5956544225751523</v>
       </c>
       <c r="E12" s="5">
@@ -801,8 +916,17 @@
       <c r="H12" s="13">
         <v>0.28449999999999998</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I12">
+        <v>124.1</v>
+      </c>
+      <c r="J12">
+        <v>91.43</v>
+      </c>
+      <c r="K12">
+        <v>1.304293636383965</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -813,7 +937,7 @@
         <v>175199</v>
       </c>
       <c r="D13" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>6.7294904651282259</v>
       </c>
       <c r="E13" s="5">
@@ -828,8 +952,17 @@
       <c r="H13" s="13">
         <v>0.29699999999999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I13">
+        <v>124.2</v>
+      </c>
+      <c r="J13">
+        <v>90.95</v>
+      </c>
+      <c r="K13">
+        <v>1.300199238282332</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -840,7 +973,7 @@
         <v>166950</v>
       </c>
       <c r="D14" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>7.2596585804132978</v>
       </c>
       <c r="E14" s="5">
@@ -855,8 +988,17 @@
       <c r="H14" s="13">
         <v>0.30480000000000002</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I14">
+        <v>124.8</v>
+      </c>
+      <c r="J14">
+        <v>90.35</v>
+      </c>
+      <c r="K14">
+        <v>1.2933056039947808</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
@@ -867,7 +1009,7 @@
         <v>165691</v>
       </c>
       <c r="D15" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>7.0613370671913378</v>
       </c>
       <c r="E15" s="5">
@@ -882,8 +1024,17 @@
       <c r="H15" s="13">
         <v>0.29320000000000002</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I15">
+        <v>124.9</v>
+      </c>
+      <c r="J15">
+        <v>91.21</v>
+      </c>
+      <c r="K15">
+        <v>1.3000565230708463</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
@@ -894,7 +1045,7 @@
         <v>162823</v>
       </c>
       <c r="D16" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>6.9216265515314177</v>
       </c>
       <c r="E16" s="5">
@@ -909,8 +1060,17 @@
       <c r="H16" s="13">
         <v>0.28050000000000003</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I16">
+        <v>124.8</v>
+      </c>
+      <c r="J16">
+        <v>91.77</v>
+      </c>
+      <c r="K16">
+        <v>1.3012828505797902</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
@@ -921,7 +1081,7 @@
         <v>158950</v>
       </c>
       <c r="D17" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>6.8134633532557407</v>
       </c>
       <c r="E17" s="5">
@@ -936,8 +1096,17 @@
       <c r="H17" s="13">
         <v>0.26800000000000002</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I17">
+        <v>124.7</v>
+      </c>
+      <c r="J17">
+        <v>92.11</v>
+      </c>
+      <c r="K17">
+        <v>1.3039279244871131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>1</v>
       </c>
@@ -948,7 +1117,7 @@
         <v>137276</v>
       </c>
       <c r="D18" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>5.8447798595530172</v>
       </c>
       <c r="E18" s="5">
@@ -963,8 +1132,17 @@
       <c r="H18" s="13">
         <v>0.19239999999999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I18">
+        <v>124.3</v>
+      </c>
+      <c r="J18">
+        <v>95.53</v>
+      </c>
+      <c r="K18">
+        <v>1.3241836764275667</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>1</v>
       </c>
@@ -975,7 +1153,7 @@
         <v>134061</v>
       </c>
       <c r="D19" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>5.7008376783702941</v>
       </c>
       <c r="E19" s="5">
@@ -990,8 +1168,17 @@
       <c r="H19" s="13">
         <v>0.1827</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I19">
+        <v>124.2</v>
+      </c>
+      <c r="J19">
+        <v>95.92</v>
+      </c>
+      <c r="K19">
+        <v>1.3276792910158586</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>1</v>
       </c>
@@ -1002,7 +1189,7 @@
         <v>131392</v>
       </c>
       <c r="D20" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>5.5415093765221624</v>
       </c>
       <c r="E20" s="5">
@@ -1017,8 +1204,17 @@
       <c r="H20" s="13">
         <v>0.17330000000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I20">
+        <v>124.2</v>
+      </c>
+      <c r="J20">
+        <v>96.3</v>
+      </c>
+      <c r="K20">
+        <v>1.3294529188860607</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>1</v>
       </c>
@@ -1029,7 +1225,7 @@
         <v>130039</v>
       </c>
       <c r="D21" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>5.3357992602219335</v>
       </c>
       <c r="E21" s="5">
@@ -1044,8 +1240,17 @@
       <c r="H21" s="13">
         <v>0.1643</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I21">
+        <v>124</v>
+      </c>
+      <c r="J21">
+        <v>96.8</v>
+      </c>
+      <c r="K21">
+        <v>1.3287291644819932</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>1</v>
       </c>
@@ -1056,7 +1261,7 @@
         <v>122343</v>
       </c>
       <c r="D22" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>5.0939571532494705</v>
       </c>
       <c r="E22" s="5">
@@ -1071,8 +1276,17 @@
       <c r="H22" s="13">
         <v>0.14319999999999999</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I22">
+        <v>123.8</v>
+      </c>
+      <c r="J22">
+        <v>97.46</v>
+      </c>
+      <c r="K22">
+        <v>1.3024143883315895</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>1</v>
       </c>
@@ -1083,7 +1297,7 @@
         <v>120309</v>
       </c>
       <c r="D23" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>4.9229567197798998</v>
       </c>
       <c r="E23" s="5">
@@ -1098,8 +1312,17 @@
       <c r="H23" s="13">
         <v>0.13569999999999999</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I23">
+        <v>123.8</v>
+      </c>
+      <c r="J23">
+        <v>97.61</v>
+      </c>
+      <c r="K23">
+        <v>1.3046654793095758</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>1</v>
       </c>
@@ -1110,7 +1333,7 @@
         <v>120691</v>
       </c>
       <c r="D24" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>4.661507486059441</v>
       </c>
       <c r="E24" s="6">
@@ -1125,8 +1348,17 @@
       <c r="H24" s="14">
         <v>0.12759999999999999</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I24">
+        <v>123.7</v>
+      </c>
+      <c r="J24">
+        <v>98.12</v>
+      </c>
+      <c r="K24">
+        <v>1.2967196544969048</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>1</v>
       </c>
@@ -1137,7 +1369,7 @@
         <v>218790</v>
       </c>
       <c r="D25" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>4.3465834818775999</v>
       </c>
       <c r="E25" s="5">
@@ -1152,8 +1384,17 @@
       <c r="H25" s="13">
         <v>0.2878</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I25">
+        <v>124.2</v>
+      </c>
+      <c r="J25">
+        <v>97.81</v>
+      </c>
+      <c r="K25">
+        <v>1.0860786872593107</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>1</v>
       </c>
@@ -1164,7 +1405,7 @@
         <v>218613</v>
       </c>
       <c r="D26" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>4.1899521071482484</v>
       </c>
       <c r="E26" s="5">
@@ -1179,8 +1420,17 @@
       <c r="H26" s="13">
         <v>0.27510000000000001</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I26">
+        <v>124.2</v>
+      </c>
+      <c r="J26">
+        <v>98.83</v>
+      </c>
+      <c r="K26">
+        <v>1.0843644365667071</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>1</v>
       </c>
@@ -1191,7 +1441,7 @@
         <v>215851</v>
       </c>
       <c r="D27" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>4.0692329430950052</v>
       </c>
       <c r="E27" s="5">
@@ -1206,8 +1456,17 @@
       <c r="H27" s="13">
         <v>0.26229999999999998</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I27">
+        <v>124.1</v>
+      </c>
+      <c r="J27">
+        <v>99.65</v>
+      </c>
+      <c r="K27">
+        <v>1.0846737410790399</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>1</v>
       </c>
@@ -1218,7 +1477,7 @@
         <v>208862</v>
       </c>
       <c r="D28" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>4.0160823893288393</v>
       </c>
       <c r="E28" s="5">
@@ -1233,8 +1492,17 @@
       <c r="H28" s="13">
         <v>0.24890000000000001</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I28">
+        <v>124</v>
+      </c>
+      <c r="J28">
+        <v>100.2</v>
+      </c>
+      <c r="K28">
+        <v>1.0844811548551307</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>1</v>
       </c>
@@ -1245,7 +1513,7 @@
         <v>205541</v>
       </c>
       <c r="D29" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3.9051235519920602</v>
       </c>
       <c r="E29" s="5">
@@ -1260,8 +1528,17 @@
       <c r="H29" s="13">
         <v>0.23699999999999999</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I29">
+        <v>123.8</v>
+      </c>
+      <c r="J29">
+        <v>100.9</v>
+      </c>
+      <c r="K29">
+        <v>1.0847160528333675</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>1</v>
       </c>
@@ -1272,7 +1549,7 @@
         <v>204387</v>
       </c>
       <c r="D30" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3.7686594548576964</v>
       </c>
       <c r="E30" s="5">
@@ -1287,8 +1564,17 @@
       <c r="H30" s="13">
         <v>0.224</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I30">
+        <v>123.8</v>
+      </c>
+      <c r="J30">
+        <v>102.2</v>
+      </c>
+      <c r="K30">
+        <v>1.0739435532163788</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>1</v>
       </c>
@@ -1299,7 +1585,7 @@
         <v>197608</v>
       </c>
       <c r="D31" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3.7055635399376543</v>
       </c>
       <c r="E31" s="5">
@@ -1314,8 +1600,17 @@
       <c r="H31" s="13">
         <v>0.2122</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I31">
+        <v>123.9</v>
+      </c>
+      <c r="J31">
+        <v>103</v>
+      </c>
+      <c r="K31">
+        <v>1.0770629569148464</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>1</v>
       </c>
@@ -1326,7 +1621,7 @@
         <v>152022</v>
       </c>
       <c r="D32" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>6.7095551959584796</v>
       </c>
       <c r="E32" s="5">
@@ -1341,8 +1636,17 @@
       <c r="H32" s="13">
         <v>0.30909999999999999</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I32">
+        <v>124.1</v>
+      </c>
+      <c r="J32">
+        <v>87.43</v>
+      </c>
+      <c r="K32">
+        <v>1.0738528843362889</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>1</v>
       </c>
@@ -1353,7 +1657,7 @@
         <v>150055</v>
       </c>
       <c r="D33" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>6.5217353636999764</v>
       </c>
       <c r="E33" s="5">
@@ -1368,8 +1672,17 @@
       <c r="H33" s="13">
         <v>0.29459999999999997</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I33">
+        <v>124</v>
+      </c>
+      <c r="J33">
+        <v>87.99</v>
+      </c>
+      <c r="K33">
+        <v>1.0742269907249691</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>1</v>
       </c>
@@ -1380,7 +1693,7 @@
         <v>148265</v>
       </c>
       <c r="D34" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>6.2916669476950053</v>
       </c>
       <c r="E34" s="5">
@@ -1395,8 +1708,17 @@
       <c r="H34" s="13">
         <v>0.27879999999999999</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I34">
+        <v>123.8</v>
+      </c>
+      <c r="J34">
+        <v>88.75</v>
+      </c>
+      <c r="K34">
+        <v>1.0742147474632573</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>1</v>
       </c>
@@ -1407,7 +1729,7 @@
         <v>146956</v>
       </c>
       <c r="D35" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>6.0907482511772235</v>
       </c>
       <c r="E35" s="5">
@@ -1422,8 +1744,17 @@
       <c r="H35" s="13">
         <v>0.2661</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I35">
+        <v>123.7</v>
+      </c>
+      <c r="J35">
+        <v>89.45</v>
+      </c>
+      <c r="K35">
+        <v>1.0750647329750878</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>1</v>
       </c>
@@ -1434,7 +1765,7 @@
         <v>144691</v>
       </c>
       <c r="D36" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>5.9264432480251017</v>
       </c>
       <c r="E36" s="5">
@@ -1449,8 +1780,17 @@
       <c r="H36" s="13">
         <v>0.2535</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I36">
+        <v>123.9</v>
+      </c>
+      <c r="J36">
+        <v>90.36</v>
+      </c>
+      <c r="K36">
+        <v>1.0766763059631677</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>1</v>
       </c>
@@ -1461,7 +1801,7 @@
         <v>144702</v>
       </c>
       <c r="D37" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>5.6872468936158453</v>
       </c>
       <c r="E37" s="5">
@@ -1476,8 +1816,17 @@
       <c r="H37" s="13">
         <v>0.24199999999999999</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I37">
+        <v>123.8</v>
+      </c>
+      <c r="J37">
+        <v>91.15</v>
+      </c>
+      <c r="K37">
+        <v>1.0767090734318656</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>1</v>
       </c>
@@ -1488,7 +1837,7 @@
         <v>143127</v>
       </c>
       <c r="D38" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>5.4995772984831657</v>
       </c>
       <c r="E38" s="5">
@@ -1503,8 +1852,17 @@
       <c r="H38" s="13">
         <v>0.23039999999999999</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I38">
+        <v>123.8</v>
+      </c>
+      <c r="J38">
+        <v>92</v>
+      </c>
+      <c r="K38">
+        <v>1.0780177638662769</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>1</v>
       </c>
@@ -1515,7 +1873,7 @@
         <v>140348</v>
       </c>
       <c r="D39" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>5.3465742297717105</v>
       </c>
       <c r="E39" s="5">
@@ -1530,8 +1888,17 @@
       <c r="H39" s="13">
         <v>0.2195</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I39">
+        <v>123.6</v>
+      </c>
+      <c r="J39">
+        <v>92.61</v>
+      </c>
+      <c r="K39">
+        <v>1.0828931051688668</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>1</v>
       </c>
@@ -1542,7 +1909,7 @@
         <v>138000</v>
       </c>
       <c r="D40" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>5.18404347826087</v>
       </c>
       <c r="E40" s="5">
@@ -1557,8 +1924,17 @@
       <c r="H40" s="13">
         <v>0.20760000000000001</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I40">
+        <v>124</v>
+      </c>
+      <c r="J40">
+        <v>93.62</v>
+      </c>
+      <c r="K40">
+        <v>1.0817747036795087</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>1</v>
       </c>
@@ -1569,7 +1945,7 @@
         <v>136890</v>
       </c>
       <c r="D41" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>4.9751625392651038</v>
       </c>
       <c r="E41" s="5">
@@ -1584,8 +1960,17 @@
       <c r="H41" s="13">
         <v>0.1973</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I41">
+        <v>123.9</v>
+      </c>
+      <c r="J41">
+        <v>94.49</v>
+      </c>
+      <c r="K41">
+        <v>1.0853260688795687</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>1</v>
       </c>
@@ -1596,7 +1981,7 @@
         <v>170956</v>
       </c>
       <c r="D42" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>6.2589204239687408</v>
       </c>
       <c r="E42" s="5">
@@ -1611,8 +1996,17 @@
       <c r="H42" s="13">
         <v>0.3286</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I42">
+        <v>124.7</v>
+      </c>
+      <c r="J42">
+        <v>89.62</v>
+      </c>
+      <c r="K42">
+        <v>1.0812094141439954</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>1</v>
       </c>
@@ -1623,7 +2017,7 @@
         <v>174829</v>
       </c>
       <c r="D43" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>6.3490610825435141</v>
       </c>
       <c r="E43" s="5">
@@ -1638,8 +2032,17 @@
       <c r="H43" s="13">
         <v>0.34439999999999998</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I43">
+        <v>124.7</v>
+      </c>
+      <c r="J43">
+        <v>89.22</v>
+      </c>
+      <c r="K43">
+        <v>1.0842627281876247</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>1</v>
       </c>
@@ -1650,7 +2053,7 @@
         <v>181586</v>
       </c>
       <c r="D44" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>6.3385943850296833</v>
       </c>
       <c r="E44" s="5">
@@ -1665,8 +2068,17 @@
       <c r="H44" s="13">
         <v>0.3619</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I44">
+        <v>124.6</v>
+      </c>
+      <c r="J44">
+        <v>89.16</v>
+      </c>
+      <c r="K44">
+        <v>1.0897206465347136</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
         <v>1</v>
       </c>
@@ -1677,7 +2089,7 @@
         <v>188608</v>
       </c>
       <c r="D45" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>6.3252884289107563</v>
       </c>
       <c r="E45" s="7">
@@ -1692,14 +2104,23 @@
       <c r="H45" s="15">
         <v>0.37840000000000001</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I45" s="16">
+        <v>124.7</v>
+      </c>
+      <c r="J45" s="16">
+        <v>89.25</v>
+      </c>
+      <c r="K45" s="16">
+        <v>1.0908395753005302</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H46" s="5"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H47" s="5"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H48" s="5"/>
     </row>
     <row r="49" spans="8:8" x14ac:dyDescent="0.3">

</xml_diff>